<commit_message>
added precision & recall scores to deck
</commit_message>
<xml_diff>
--- a/outputs/crossValV2/precisionReport.xlsx
+++ b/outputs/crossValV2/precisionReport.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lando\Documents\GitHub\Buell-Masters-Project\outputs\crossValV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639A9AE9-C259-4897-9798-2E538CF7CF1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D1A33D-6E28-427A-B263-CD5CFBC16906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25200" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$C$32:$L$32</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -247,21 +250,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -277,6 +279,1152 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average Precision</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Score Across K = 10 Folds</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="63500">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$32:$L$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.88621512965517246</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.91886753379310326</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.93467576034482758</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.91946535172413779</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.87132540034482764</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.92613762344827577</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.89119741068965519</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.91989962206896569</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.93487454241379297</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9288593755172414</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2AFE-427A-85E2-0AABC3E67136}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="315"/>
+        <c:overlap val="-40"/>
+        <c:axId val="168862415"/>
+        <c:axId val="2006685695"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="168862415"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Fold Index</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2006685695"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2006685695"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t> Metric</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Score</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="168862415"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="213">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB80A920-BFBA-344C-EC8C-64A68E0CD66F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -544,8 +1692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -555,1487 +1703,1487 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="4" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
+      <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>0.90441179999999999</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>0.98106059999999995</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3">
         <v>0.96478872999999998</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3">
         <v>0.90634440000000005</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3">
         <v>0.88435375999999999</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3">
         <v>0.89189189999999996</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3">
         <v>0.91752577000000002</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3">
         <v>0.87748340000000002</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3">
         <v>0.9291045</v>
       </c>
       <c r="L3">
         <v>0.94648829999999995</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="2">
         <f>AVERAGE(C3:L3)</f>
         <v>0.92034531600000002</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="2">
         <f>VAR(C3:M3)</f>
         <v>1.0821726925114828E-3</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>0.87812500000000004</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>0.98239434000000003</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4">
         <v>0.98671096999999997</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
         <v>0.93225807000000005</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4">
         <v>0.90068495000000004</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4">
         <v>0.95238096000000005</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4">
         <v>0.80459769999999997</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4">
         <v>0.97945210000000005</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4">
         <v>0.97037035000000005</v>
       </c>
       <c r="L4">
         <v>0.94927539999999999</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="2">
         <f t="shared" ref="M4:M31" si="0">AVERAGE(C4:L4)</f>
         <v>0.93362498399999994</v>
       </c>
-      <c r="N4" s="5">
-        <f t="shared" ref="N4:N33" si="1">VAR(C4:M4)</f>
+      <c r="N4" s="2">
+        <f t="shared" ref="N4:N31" si="1">VAR(C4:M4)</f>
         <v>3.0058843168505444E-3</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>0.94983280000000003</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>0.97627120000000001</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5">
         <v>0.99358975999999999</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5">
         <v>0.95737709999999998</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5">
         <v>0.94545453999999995</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5">
         <v>1</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5">
         <v>0.95847749999999998</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5">
         <v>0.98634814999999998</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5">
         <v>0.99672130000000003</v>
       </c>
       <c r="L5">
         <v>0.99681525999999998</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="2">
         <f t="shared" si="0"/>
         <v>0.97608876100000008</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="2">
         <f t="shared" si="1"/>
         <v>4.1267238452380917E-4</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>0.81375359999999997</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>0.9766667</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6">
         <v>0.94267520000000005</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6">
         <v>0.95859872999999995</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6">
         <v>0.95019156000000005</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6">
         <v>0.94212216000000004</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6">
         <v>0.9425287</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6">
         <v>0.96153843000000006</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6">
         <v>0.95043730000000004</v>
       </c>
       <c r="L6">
         <v>0.88349515000000001</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="2">
         <f t="shared" si="0"/>
         <v>0.93220075300000005</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="2">
         <f t="shared" si="1"/>
         <v>2.0907792370499423E-3</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="3">
+      <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>0.84899329999999995</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <v>0.94964029999999999</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7">
         <v>0.82240440000000004</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7">
         <v>0.87632509999999997</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7">
         <v>0.7051887</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7">
         <v>0.86738353999999995</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7">
         <v>0.78012049999999999</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7">
         <v>0.93333334000000001</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7">
         <v>0.90181816000000004</v>
       </c>
       <c r="L7">
         <v>0.86619716999999996</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="2">
         <f t="shared" si="0"/>
         <v>0.85514045099999991</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="2">
         <f t="shared" si="1"/>
         <v>4.7167048661737685E-3</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="3">
+      <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>0.92465750000000002</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <v>0.92459020000000003</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8">
         <v>0.96226420000000001</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8">
         <v>0.942492</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8">
         <v>0.95599999999999996</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8">
         <v>0.97712414999999997</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8">
         <v>0.83898306</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8">
         <v>0.98045605000000002</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8">
         <v>0.9728097</v>
       </c>
       <c r="L8">
         <v>0.9773463</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="2">
         <f t="shared" si="0"/>
         <v>0.94567231600000012</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="2">
         <f t="shared" si="1"/>
         <v>1.6599546419460039E-3</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="3">
+      <c r="A9" s="1">
         <v>6</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>0.94626869999999996</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9">
         <v>0.98688525000000005</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9">
         <v>0.91780823</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9">
         <v>0.96453900000000004</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9">
         <v>0.85624999999999996</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9">
         <v>0.94461536000000002</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9">
         <v>0.9353612</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9">
         <v>0.92682929999999997</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9">
         <v>0.92361110000000002</v>
       </c>
       <c r="L9">
         <v>0.98076920000000001</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="2">
         <f t="shared" si="0"/>
         <v>0.93829373399999993</v>
       </c>
-      <c r="N9" s="5">
+      <c r="N9" s="2">
         <f t="shared" si="1"/>
         <v>1.2464120571067452E-3</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
+      <c r="A10" s="1">
         <v>7</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <v>0.95945950000000002</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10">
         <v>0.95637583999999998</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10">
         <v>0.99315070000000005</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10">
         <v>0.92880260000000003</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10">
         <v>0.93870969999999998</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10">
         <v>0.97419359999999999</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10">
         <v>0.87658225999999995</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10">
         <v>0.91614910000000005</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10">
         <v>0.97770699999999999</v>
       </c>
       <c r="L10">
         <v>0.97009970000000001</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="2">
         <f t="shared" si="0"/>
         <v>0.94912299999999994</v>
       </c>
-      <c r="N10" s="5">
+      <c r="N10" s="2">
         <f t="shared" si="1"/>
         <v>1.0854279784863208E-3</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="3">
+      <c r="A11" s="1">
         <v>8</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11">
         <v>0.81791910000000001</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11">
         <v>0.75218660000000004</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11">
         <v>0.9375</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11">
         <v>0.96699670000000004</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11">
         <v>0.75749319999999998</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11">
         <v>0.90228014999999995</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11">
         <v>0.94080997</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11">
         <v>0.89354836999999998</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11">
         <v>0.87628865</v>
       </c>
       <c r="L11">
         <v>0.96258502999999995</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M11" s="2">
         <f t="shared" si="0"/>
         <v>0.88076077700000011</v>
       </c>
-      <c r="N11" s="5">
+      <c r="N11" s="2">
         <f t="shared" si="1"/>
         <v>5.7278984569066414E-3</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="3">
+      <c r="A12" s="1">
         <v>9</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>0.96453900000000004</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12">
         <v>0.93290733999999997</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12">
         <v>0.95294120000000004</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12">
         <v>0.97938144000000005</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12">
         <v>0.91512910000000003</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12">
         <v>0.96336997000000002</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12">
         <v>0.94964029999999999</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12">
         <v>0.93769469999999999</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12">
         <v>0.96989965</v>
       </c>
       <c r="L12">
         <v>0.98722047000000002</v>
       </c>
-      <c r="M12" s="5">
+      <c r="M12" s="2">
         <f t="shared" si="0"/>
         <v>0.95527231700000015</v>
       </c>
-      <c r="N12" s="5">
+      <c r="N12" s="2">
         <f t="shared" si="1"/>
         <v>4.4251329692386132E-4</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="3">
+      <c r="A13" s="1">
         <v>10</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>0.875</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13">
         <v>0.89032257000000004</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13">
         <v>0.87570619999999999</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13">
         <v>0.93421054000000003</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13">
         <v>0.8302583</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13">
         <v>0.82758622999999998</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13">
         <v>0.94035089999999999</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13">
         <v>0.80113639999999997</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13">
         <v>0.91946309999999998</v>
       </c>
       <c r="L13">
         <v>0.956229</v>
       </c>
-      <c r="M13" s="5">
+      <c r="M13" s="2">
         <f t="shared" si="0"/>
         <v>0.88502632400000003</v>
       </c>
-      <c r="N13" s="5">
+      <c r="N13" s="2">
         <f t="shared" si="1"/>
         <v>2.5287470730289648E-3</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="3">
+      <c r="A14" s="1">
         <v>11</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>0.9572368</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14">
         <v>0.95283019999999996</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14">
         <v>0.98344374000000001</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14">
         <v>0.97132620000000003</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14">
         <v>0.97894734000000005</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14">
         <v>0.96923079999999995</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I14">
         <v>0.93225807000000005</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14">
         <v>0.96140349999999997</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14">
         <v>0.94385964</v>
       </c>
       <c r="L14">
         <v>0.97972970000000004</v>
       </c>
-      <c r="M14" s="5">
+      <c r="M14" s="2">
         <f t="shared" si="0"/>
         <v>0.96302659900000021</v>
       </c>
-      <c r="N14" s="5">
+      <c r="N14" s="2">
         <f t="shared" si="1"/>
         <v>2.5108961799496908E-4</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="3">
+      <c r="A15" s="1">
         <v>12</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>0.91566265000000002</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15">
         <v>0.84593019999999997</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15">
         <v>0.86969700000000005</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15">
         <v>0.90425533000000002</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15">
         <v>0.81848186000000001</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15">
         <v>0.9</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15">
         <v>0.93385214000000005</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15">
         <v>0.84918033999999998</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15">
         <v>0.84340660000000001</v>
       </c>
       <c r="L15">
         <v>0.86759580000000003</v>
       </c>
-      <c r="M15" s="5">
+      <c r="M15" s="2">
         <f t="shared" si="0"/>
         <v>0.87480619199999998</v>
       </c>
-      <c r="N15" s="5">
+      <c r="N15" s="2">
         <f t="shared" si="1"/>
         <v>1.2384619379417574E-3</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="3">
+      <c r="A16" s="1">
         <v>13</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
         <v>0.81884056000000005</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16">
         <v>0.94139194000000004</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16">
         <v>0.96551719999999996</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16">
         <v>0.93644070000000001</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16">
         <v>0.79213480000000003</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16">
         <v>0.83008355</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16">
         <v>0.87861270000000002</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16">
         <v>0.95864660000000002</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16">
         <v>0.94539249999999997</v>
       </c>
       <c r="L16">
         <v>0.90459365000000003</v>
       </c>
-      <c r="M16" s="5">
+      <c r="M16" s="2">
         <f t="shared" si="0"/>
         <v>0.8971654200000001</v>
       </c>
-      <c r="N16" s="5">
+      <c r="N16" s="2">
         <f t="shared" si="1"/>
         <v>3.6341859393708175E-3</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" s="3">
+      <c r="A17" s="1">
         <v>14</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>0.80440769999999995</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17">
         <v>0.95131089999999996</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17">
         <v>0.93283579999999999</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17">
         <v>0.81578945999999997</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17">
         <v>0.91864409999999996</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17">
         <v>0.91437310000000005</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17">
         <v>0.87707639999999998</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J17">
         <v>0.90909094000000001</v>
       </c>
-      <c r="K17" s="1">
+      <c r="K17">
         <v>0.93425610000000003</v>
       </c>
       <c r="L17">
         <v>0.92880260000000003</v>
       </c>
-      <c r="M17" s="5">
+      <c r="M17" s="2">
         <f t="shared" si="0"/>
         <v>0.89865871000000008</v>
       </c>
-      <c r="N17" s="5">
+      <c r="N17" s="2">
         <f t="shared" si="1"/>
         <v>2.3087705747624216E-3</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" s="3">
+      <c r="A18" s="1">
         <v>15</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
         <v>0.94065284999999998</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18">
         <v>0.95409834000000004</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18">
         <v>0.99230766000000004</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18">
         <v>0.9055375</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18">
         <v>0.89368769999999997</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18">
         <v>0.94863014999999995</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18">
         <v>0.91349480000000005</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J18">
         <v>0.96116509999999999</v>
       </c>
-      <c r="K18" s="1">
+      <c r="K18">
         <v>0.9833887</v>
       </c>
       <c r="L18">
         <v>0.97435899999999998</v>
       </c>
-      <c r="M18" s="5">
+      <c r="M18" s="2">
         <f t="shared" si="0"/>
         <v>0.94673217999999992</v>
       </c>
-      <c r="N18" s="5">
+      <c r="N18" s="2">
         <f t="shared" si="1"/>
         <v>1.0102638003332202E-3</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" s="3">
+      <c r="A19" s="1">
         <v>16</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
         <v>0.95698919999999998</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19">
         <v>0.98107255000000004</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19">
         <v>0.96563569999999999</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19">
         <v>0.97212540000000003</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19">
         <v>0.97491039999999995</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19">
         <v>0.95438593999999999</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I19">
         <v>0.95394736999999996</v>
       </c>
-      <c r="J19" s="1">
+      <c r="J19">
         <v>0.99322029999999994</v>
       </c>
-      <c r="K19" s="1">
+      <c r="K19">
         <v>0.98344374000000001</v>
       </c>
       <c r="L19">
         <v>0.92260059999999999</v>
       </c>
-      <c r="M19" s="5">
+      <c r="M19" s="2">
         <f t="shared" si="0"/>
         <v>0.96583311999999988</v>
       </c>
-      <c r="N19" s="5">
+      <c r="N19" s="2">
         <f t="shared" si="1"/>
         <v>3.6340352558466004E-4</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" s="3">
+      <c r="A20" s="1">
         <v>17</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20">
         <v>0.81972789999999995</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20">
         <v>0.83838385000000004</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20">
         <v>0.88023954999999998</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20">
         <v>0.90842489999999998</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20">
         <v>0.87654319999999997</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20">
         <v>0.88571429999999995</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I20">
         <v>0.86899559999999998</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J20">
         <v>0.94693875000000005</v>
       </c>
-      <c r="K20" s="1">
+      <c r="K20">
         <v>0.93023259999999997</v>
       </c>
       <c r="L20">
         <v>0.77384200000000003</v>
       </c>
-      <c r="M20" s="5">
+      <c r="M20" s="2">
         <f t="shared" si="0"/>
         <v>0.87290426500000007</v>
       </c>
-      <c r="N20" s="5">
+      <c r="N20" s="2">
         <f t="shared" si="1"/>
         <v>2.4108498579955245E-3</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" s="3">
+      <c r="A21" s="1">
         <v>18</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21">
         <v>0.81205669999999996</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21">
         <v>0.85829960000000005</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21">
         <v>0.88235295000000002</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21">
         <v>0.78816200000000003</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21">
         <v>0.86311789999999999</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21">
         <v>0.88333329999999999</v>
       </c>
-      <c r="I21" s="1">
+      <c r="I21">
         <v>0.91029899999999997</v>
       </c>
-      <c r="J21" s="1">
+      <c r="J21">
         <v>0.93140789999999996</v>
       </c>
-      <c r="K21" s="1">
+      <c r="K21">
         <v>0.93772893999999996</v>
       </c>
       <c r="L21">
         <v>0.91007196999999995</v>
       </c>
-      <c r="M21" s="5">
+      <c r="M21" s="2">
         <f t="shared" si="0"/>
         <v>0.87768302600000003</v>
       </c>
-      <c r="N21" s="5">
+      <c r="N21" s="2">
         <f t="shared" si="1"/>
         <v>2.1567141973500223E-3</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A22" s="3">
+      <c r="A22" s="1">
         <v>19</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22">
         <v>0.8433735</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22">
         <v>0.92628204999999997</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22">
         <v>0.89354836999999998</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22">
         <v>0.87605630000000001</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22">
         <v>0.8512111</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22">
         <v>0.92255889999999996</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I22">
         <v>0.90066223999999995</v>
       </c>
-      <c r="J22" s="1">
+      <c r="J22">
         <v>0.94897960000000003</v>
       </c>
-      <c r="K22" s="1">
+      <c r="K22">
         <v>0.92024539999999999</v>
       </c>
       <c r="L22">
         <v>0.89361703000000003</v>
       </c>
-      <c r="M22" s="5">
+      <c r="M22" s="2">
         <f t="shared" si="0"/>
         <v>0.8976534490000001</v>
       </c>
-      <c r="N22" s="5">
+      <c r="N22" s="2">
         <f t="shared" si="1"/>
         <v>1.0196486975421891E-3</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A23" s="3">
+      <c r="A23" s="1">
         <v>20</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23">
         <v>0.74592835000000002</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23">
         <v>0.82116789999999995</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23">
         <v>0.85209005999999998</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23">
         <v>0.70918369999999997</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23">
         <v>0.7770492</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H23">
         <v>0.77479889999999996</v>
       </c>
-      <c r="I23" s="1">
+      <c r="I23">
         <v>0.62929064000000001</v>
       </c>
-      <c r="J23" s="1">
+      <c r="J23">
         <v>0.85496179999999999</v>
       </c>
-      <c r="K23" s="1">
+      <c r="K23">
         <v>0.82371795000000003</v>
       </c>
       <c r="L23">
         <v>0.91505789999999998</v>
       </c>
-      <c r="M23" s="5">
+      <c r="M23" s="2">
         <f t="shared" si="0"/>
         <v>0.79032463999999991</v>
       </c>
-      <c r="N23" s="5">
+      <c r="N23" s="2">
         <f t="shared" si="1"/>
         <v>6.0521853326642189E-3</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A24" s="3">
+      <c r="A24" s="1">
         <v>21</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24">
         <v>0.76567655999999995</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24">
         <v>0.74581003000000001</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24">
         <v>0.91262140000000003</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24">
         <v>0.88692579999999999</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24">
         <v>0.73260075000000002</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H24">
         <v>0.88235295000000002</v>
       </c>
-      <c r="I24" s="1">
+      <c r="I24">
         <v>0.72477066999999995</v>
       </c>
-      <c r="J24" s="1">
+      <c r="J24">
         <v>0.84814816999999998</v>
       </c>
-      <c r="K24" s="1">
+      <c r="K24">
         <v>0.79331309999999999</v>
       </c>
       <c r="L24">
         <v>0.80061349999999998</v>
       </c>
-      <c r="M24" s="5">
+      <c r="M24" s="2">
         <f t="shared" si="0"/>
         <v>0.80928329299999979</v>
       </c>
-      <c r="N24" s="5">
+      <c r="N24" s="2">
         <f t="shared" si="1"/>
         <v>4.2839987191118827E-3</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A25" s="3">
+      <c r="A25" s="1">
         <v>22</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25">
         <v>0.93877553999999996</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25">
         <v>0.92783504999999999</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25">
         <v>0.92409240000000004</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25">
         <v>0.89967640000000004</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25">
         <v>0.88888889999999998</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H25">
         <v>0.91258740000000005</v>
       </c>
-      <c r="I25" s="1">
+      <c r="I25">
         <v>0.86851210000000001</v>
       </c>
-      <c r="J25" s="1">
+      <c r="J25">
         <v>0.82903223999999998</v>
       </c>
-      <c r="K25" s="1">
+      <c r="K25">
         <v>0.89057750000000002</v>
       </c>
       <c r="L25">
         <v>0.95744680000000004</v>
       </c>
-      <c r="M25" s="5">
+      <c r="M25" s="2">
         <f t="shared" si="0"/>
         <v>0.90374243300000001</v>
       </c>
-      <c r="N25" s="5">
+      <c r="N25" s="2">
         <f t="shared" si="1"/>
         <v>1.2417551242206817E-3</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A26" s="3">
+      <c r="A26" s="1">
         <v>23</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26">
         <v>0.81230769999999997</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26">
         <v>0.75136614000000002</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26">
         <v>0.87748340000000002</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26">
         <v>0.95918369999999997</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26">
         <v>0.77167629999999998</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H26">
         <v>0.95801526000000004</v>
       </c>
-      <c r="I26" s="1">
+      <c r="I26">
         <v>0.82954543999999997</v>
       </c>
-      <c r="J26" s="1">
+      <c r="J26">
         <v>0.83433734999999998</v>
       </c>
-      <c r="K26" s="1">
+      <c r="K26">
         <v>0.88059699999999996</v>
       </c>
       <c r="L26">
         <v>0.80681820000000004</v>
       </c>
-      <c r="M26" s="5">
+      <c r="M26" s="2">
         <f t="shared" si="0"/>
         <v>0.84813304899999997</v>
       </c>
-      <c r="N26" s="5">
+      <c r="N26" s="2">
         <f t="shared" si="1"/>
         <v>4.5057360643289291E-3</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A27" s="3">
+      <c r="A27" s="1">
         <v>24</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27">
         <v>0.87352943000000005</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27">
         <v>0.956229</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27">
         <v>0.93984959999999995</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27">
         <v>0.89045936000000003</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27">
         <v>0.91479820000000001</v>
       </c>
-      <c r="H27" s="1">
+      <c r="H27">
         <v>0.96374625000000003</v>
       </c>
-      <c r="I27" s="1">
+      <c r="I27">
         <v>0.96525097000000004</v>
       </c>
-      <c r="J27" s="1">
+      <c r="J27">
         <v>0.85958904000000003</v>
       </c>
-      <c r="K27" s="1">
+      <c r="K27">
         <v>0.95818820000000005</v>
       </c>
       <c r="L27">
         <v>0.95555555999999997</v>
       </c>
-      <c r="M27" s="5">
+      <c r="M27" s="2">
         <f t="shared" si="0"/>
         <v>0.92771956099999997</v>
       </c>
-      <c r="N27" s="5">
+      <c r="N27" s="2">
         <f t="shared" si="1"/>
         <v>1.4503258081085884E-3</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A28" s="3">
+      <c r="A28" s="1">
         <v>25</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28">
         <v>0.94693875000000005</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28">
         <v>0.94670843999999998</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28">
         <v>0.93680300000000005</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28">
         <v>0.98790323999999996</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G28">
         <v>0.89067525000000003</v>
       </c>
-      <c r="H28" s="1">
+      <c r="H28">
         <v>0.97727275000000002</v>
       </c>
-      <c r="I28" s="1">
+      <c r="I28">
         <v>0.92088610000000004</v>
       </c>
-      <c r="J28" s="1">
+      <c r="J28">
         <v>0.95937499999999998</v>
       </c>
-      <c r="K28" s="1">
+      <c r="K28">
         <v>0.99264704999999998</v>
       </c>
       <c r="L28">
         <v>0.92721520000000002</v>
       </c>
-      <c r="M28" s="5">
+      <c r="M28" s="2">
         <f t="shared" si="0"/>
         <v>0.94864247800000001</v>
       </c>
-      <c r="N28" s="5">
+      <c r="N28" s="2">
         <f t="shared" si="1"/>
         <v>9.1492500085663488E-4</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A29" s="3">
+      <c r="A29" s="1">
         <v>26</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29">
         <v>0.91562500000000002</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29">
         <v>0.98897060000000003</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29">
         <v>0.99312716999999995</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29">
         <v>0.95571952999999998</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G29">
         <v>0.79439249999999995</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H29">
         <v>0.97953219999999996</v>
       </c>
-      <c r="I29" s="1">
+      <c r="I29">
         <v>0.89399295999999995</v>
       </c>
-      <c r="J29" s="1">
+      <c r="J29">
         <v>0.85519122999999997</v>
       </c>
-      <c r="K29" s="1">
+      <c r="K29">
         <v>0.96917810000000004</v>
       </c>
       <c r="L29">
         <v>0.95593220000000001</v>
       </c>
-      <c r="M29" s="5">
+      <c r="M29" s="2">
         <f t="shared" si="0"/>
         <v>0.93016614899999994</v>
       </c>
-      <c r="N29" s="5">
+      <c r="N29" s="2">
         <f t="shared" si="1"/>
         <v>3.8273524458102303E-3</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A30" s="3">
+      <c r="A30" s="1">
         <v>27</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30">
         <v>0.96232879999999998</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30">
         <v>0.95774649999999995</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30">
         <v>0.95759720000000004</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F30">
         <v>0.95</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G30">
         <v>0.93197280000000005</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H30">
         <v>0.96511625999999995</v>
       </c>
-      <c r="I30" s="1">
+      <c r="I30">
         <v>0.96850395</v>
       </c>
-      <c r="J30" s="1">
+      <c r="J30">
         <v>0.98920863999999997</v>
       </c>
-      <c r="K30" s="1">
+      <c r="K30">
         <v>0.9929578</v>
       </c>
       <c r="L30">
         <v>0.98979589999999995</v>
       </c>
-      <c r="M30" s="5">
+      <c r="M30" s="2">
         <f t="shared" si="0"/>
         <v>0.96652278500000011</v>
       </c>
-      <c r="N30" s="5">
+      <c r="N30" s="2">
         <f t="shared" si="1"/>
         <v>3.4019818880974458E-4</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A31" s="3">
+      <c r="A31" s="1">
         <v>28</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31">
         <v>0.98722047000000002</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31">
         <v>0.99242425000000001</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E31">
         <v>0.99681525999999998</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F31">
         <v>1</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G31">
         <v>0.95899049999999997</v>
       </c>
-      <c r="H31" s="1">
+      <c r="H31">
         <v>0.99331104999999997</v>
       </c>
-      <c r="I31" s="1">
+      <c r="I31">
         <v>0.98979589999999995</v>
       </c>
-      <c r="J31" s="1">
+      <c r="J31">
         <v>0.99324319999999999</v>
       </c>
-      <c r="K31" s="1">
+      <c r="K31">
         <v>1</v>
       </c>
       <c r="L31">
         <v>0.99675329999999995</v>
       </c>
-      <c r="M31" s="5">
+      <c r="M31" s="2">
         <f t="shared" si="0"/>
         <v>0.99085539300000003</v>
       </c>
-      <c r="N31" s="5">
+      <c r="N31" s="2">
         <f t="shared" si="1"/>
         <v>1.2814527783990107E-4</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="7">
+      <c r="B32" s="5"/>
+      <c r="C32" s="3">
         <f>AVERAGE(C3:C31)</f>
         <v>0.88621512965517246</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="3">
         <f t="shared" ref="D32:L32" si="2">AVERAGE(D3:D31)</f>
         <v>0.91886753379310326</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="3">
         <f t="shared" si="2"/>
         <v>0.93467576034482758</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="3">
         <f t="shared" si="2"/>
         <v>0.91946535172413779</v>
       </c>
-      <c r="G32" s="7">
+      <c r="G32" s="3">
         <f t="shared" si="2"/>
         <v>0.87132540034482764</v>
       </c>
-      <c r="H32" s="7">
+      <c r="H32" s="3">
         <f t="shared" si="2"/>
         <v>0.92613762344827577</v>
       </c>
-      <c r="I32" s="7">
+      <c r="I32" s="3">
         <f t="shared" si="2"/>
         <v>0.89119741068965519</v>
       </c>
-      <c r="J32" s="7">
+      <c r="J32" s="3">
         <f t="shared" si="2"/>
         <v>0.91989962206896569</v>
       </c>
-      <c r="K32" s="7">
+      <c r="K32" s="3">
         <f t="shared" si="2"/>
         <v>0.93487454241379297</v>
       </c>
-      <c r="L32" s="7">
+      <c r="L32" s="3">
         <f t="shared" si="2"/>
         <v>0.9288593755172414</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="7">
+      <c r="B33" s="5"/>
+      <c r="C33" s="3">
         <f>VAR(C3:C32)</f>
         <v>4.5678609982933499E-3</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="3">
         <f t="shared" ref="D33:L33" si="3">VAR(D3:D32)</f>
         <v>5.3562362986067872E-3</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="3">
         <f t="shared" si="3"/>
         <v>2.268620487849789E-3</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="3">
         <f t="shared" si="3"/>
         <v>3.8467884067308281E-3</v>
       </c>
-      <c r="G33" s="7">
+      <c r="G33" s="3">
         <f t="shared" si="3"/>
         <v>5.5648377443999137E-3</v>
       </c>
-      <c r="H33" s="7">
+      <c r="H33" s="3">
         <f t="shared" si="3"/>
         <v>2.881480589418243E-3</v>
       </c>
-      <c r="I33" s="7">
+      <c r="I33" s="3">
         <f t="shared" si="3"/>
         <v>5.9586457407872339E-3</v>
       </c>
-      <c r="J33" s="7">
+      <c r="J33" s="3">
         <f t="shared" si="3"/>
         <v>3.1778954810991415E-3</v>
       </c>
-      <c r="K33" s="7">
+      <c r="K33" s="3">
         <f t="shared" si="3"/>
         <v>2.6979784844533357E-3</v>
       </c>
-      <c r="L33" s="7">
+      <c r="L33" s="3">
         <f t="shared" si="3"/>
         <v>3.4535698429444582E-3</v>
       </c>
@@ -2050,5 +3198,6 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>